<commit_message>
Latest version w working  hh_edu and disability
</commit_message>
<xml_diff>
--- a/wide_pipeline/dhs_dictionary_setcode.xlsx
+++ b/wide_pipeline/dhs_dictionary_setcode.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\personal\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F888F3C8-1B78-4DAB-82EF-3EC5625E4F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dictionary" sheetId="1" r:id="rId1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="663">
   <si>
     <t>name</t>
   </si>
@@ -2021,12 +2022,15 @@
   </si>
   <si>
     <t>label was 2002, but the value said 2</t>
+  </si>
+  <si>
+    <t>hv101</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -2340,16 +2344,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2366,7 +2370,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2374,7 +2378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2382,7 +2386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2390,7 +2394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -2401,7 +2405,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -2409,7 +2413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -2417,7 +2421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -2428,7 +2432,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -2436,7 +2440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -2444,7 +2448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -2452,7 +2456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -2460,7 +2464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -2468,7 +2472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -2482,7 +2486,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -2493,7 +2497,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -2504,140 +2508,149 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>662</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D27" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D28" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D31" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D33" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2652,22 +2665,22 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.08984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" style="1" customWidth="1"/>
-    <col min="3" max="64" width="8.1796875" customWidth="1"/>
-    <col min="65" max="1024" width="10.54296875" style="1"/>
+    <col min="1" max="1" width="6.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="1" customWidth="1"/>
+    <col min="3" max="64" width="8.140625" customWidth="1"/>
+    <col min="65" max="1024" width="10.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -2675,7 +2688,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>8</v>
       </c>
@@ -2683,7 +2696,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>9</v>
       </c>
@@ -2702,23 +2715,23 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AMJ5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="6.08984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" style="1" customWidth="1"/>
-    <col min="5" max="64" width="8.1796875" customWidth="1"/>
-    <col min="65" max="1024" width="10.54296875" style="1"/>
+    <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="6.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="1" customWidth="1"/>
+    <col min="5" max="64" width="8.140625" customWidth="1"/>
+    <col min="65" max="1024" width="10.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -2732,7 +2745,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>57</v>
       </c>
@@ -2746,7 +2759,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>56</v>
       </c>
@@ -2760,7 +2773,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
@@ -2774,7 +2787,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>53</v>
       </c>
@@ -2799,24 +2812,24 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AMJ7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.08984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="29" style="1" customWidth="1"/>
-    <col min="5" max="64" width="8.1796875" customWidth="1"/>
-    <col min="65" max="1024" width="10.54296875" style="1"/>
+    <col min="5" max="64" width="8.140625" customWidth="1"/>
+    <col min="65" max="1024" width="10.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -2830,7 +2843,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>655</v>
       </c>
@@ -2842,7 +2855,7 @@
       </c>
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>656</v>
       </c>
@@ -2854,7 +2867,7 @@
       </c>
       <c r="D3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>657</v>
       </c>
@@ -2866,7 +2879,7 @@
       </c>
       <c r="D4"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>658</v>
       </c>
@@ -2878,7 +2891,7 @@
       </c>
       <c r="D5"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>656</v>
       </c>
@@ -2892,7 +2905,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>660</v>
       </c>
@@ -2917,22 +2930,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" style="1" customWidth="1"/>
-    <col min="3" max="64" width="8.1796875" customWidth="1"/>
-    <col min="65" max="1024" width="10.54296875" style="1"/>
+    <col min="1" max="1" width="3.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="1" customWidth="1"/>
+    <col min="3" max="64" width="8.140625" customWidth="1"/>
+    <col min="65" max="1024" width="10.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -2940,7 +2953,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -2948,7 +2961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>9</v>
       </c>
@@ -2956,7 +2969,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2964,7 +2977,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2983,28 +2996,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.08984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="3.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.36328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.08984375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" style="1" customWidth="1"/>
-    <col min="9" max="64" width="8.1796875" customWidth="1"/>
-    <col min="65" max="1024" width="10.54296875" style="1"/>
+    <col min="1" max="1" width="7.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" style="1" customWidth="1"/>
+    <col min="9" max="64" width="8.140625" customWidth="1"/>
+    <col min="65" max="1024" width="10.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -3012,7 +3025,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -3020,7 +3033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>9</v>
       </c>
@@ -3039,23 +3052,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ60"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" style="1" customWidth="1"/>
-    <col min="4" max="64" width="8.1796875" customWidth="1"/>
-    <col min="65" max="1024" width="10.54296875" style="1"/>
+    <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="1" customWidth="1"/>
+    <col min="4" max="64" width="8.140625" customWidth="1"/>
+    <col min="65" max="1024" width="10.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -3066,7 +3079,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>49</v>
       </c>
@@ -3077,7 +3090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -3088,7 +3101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>49</v>
       </c>
@@ -3099,7 +3112,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
@@ -3110,7 +3123,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>49</v>
       </c>
@@ -3121,7 +3134,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>49</v>
       </c>
@@ -3132,7 +3145,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>50</v>
       </c>
@@ -3143,7 +3156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>50</v>
       </c>
@@ -3154,7 +3167,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>50</v>
       </c>
@@ -3165,7 +3178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
@@ -3176,7 +3189,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>50</v>
       </c>
@@ -3187,7 +3200,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
@@ -3198,7 +3211,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
@@ -3209,7 +3222,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>51</v>
       </c>
@@ -3220,7 +3233,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>51</v>
       </c>
@@ -3231,7 +3244,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>51</v>
       </c>
@@ -3242,7 +3255,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
@@ -3253,7 +3266,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>51</v>
       </c>
@@ -3264,7 +3277,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>52</v>
       </c>
@@ -3275,7 +3288,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>52</v>
       </c>
@@ -3286,7 +3299,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>52</v>
       </c>
@@ -3297,7 +3310,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>52</v>
       </c>
@@ -3308,7 +3321,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -3319,7 +3332,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>52</v>
       </c>
@@ -3330,7 +3343,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>52</v>
       </c>
@@ -3341,7 +3354,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
@@ -3352,7 +3365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>53</v>
       </c>
@@ -3363,7 +3376,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>53</v>
       </c>
@@ -3374,7 +3387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
@@ -3385,7 +3398,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>53</v>
       </c>
@@ -3396,7 +3409,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>53</v>
       </c>
@@ -3407,7 +3420,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>53</v>
       </c>
@@ -3418,7 +3431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>53</v>
       </c>
@@ -3429,7 +3442,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>53</v>
       </c>
@@ -3440,7 +3453,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>53</v>
       </c>
@@ -3451,7 +3464,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>53</v>
       </c>
@@ -3462,7 +3475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>53</v>
       </c>
@@ -3473,7 +3486,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>54</v>
       </c>
@@ -3484,7 +3497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>54</v>
       </c>
@@ -3495,7 +3508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>54</v>
       </c>
@@ -3506,7 +3519,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>54</v>
       </c>
@@ -3517,7 +3530,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>54</v>
       </c>
@@ -3528,7 +3541,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>55</v>
       </c>
@@ -3539,7 +3552,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>55</v>
       </c>
@@ -3550,7 +3563,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>55</v>
       </c>
@@ -3561,7 +3574,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>55</v>
       </c>
@@ -3572,7 +3585,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>55</v>
       </c>
@@ -3583,7 +3596,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>56</v>
       </c>
@@ -3594,7 +3607,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>56</v>
       </c>
@@ -3605,7 +3618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>56</v>
       </c>
@@ -3616,7 +3629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>56</v>
       </c>
@@ -3627,7 +3640,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>56</v>
       </c>
@@ -3638,7 +3651,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>56</v>
       </c>
@@ -3649,7 +3662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>57</v>
       </c>
@@ -3660,7 +3673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
@@ -3671,7 +3684,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>57</v>
       </c>
@@ -3682,7 +3695,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
@@ -3693,7 +3706,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
@@ -3704,7 +3717,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
@@ -3726,25 +3739,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="19.26953125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="19.28515625" style="1" customWidth="1"/>
     <col min="3" max="4" width="14" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.08984375" style="1" customWidth="1"/>
-    <col min="6" max="7" width="15.54296875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="59.36328125" style="1" customWidth="1"/>
-    <col min="9" max="66" width="8.1796875" customWidth="1"/>
-    <col min="67" max="1024" width="10.54296875" style="1"/>
+    <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="15.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="59.42578125" style="1" customWidth="1"/>
+    <col min="9" max="66" width="8.140625" customWidth="1"/>
+    <col min="67" max="1024" width="10.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>59</v>
       </c>
@@ -3770,7 +3783,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>66</v>
       </c>
@@ -3790,7 +3803,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>69</v>
       </c>
@@ -3810,7 +3823,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>72</v>
       </c>
@@ -3832,7 +3845,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>75</v>
       </c>
@@ -3856,7 +3869,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>77</v>
       </c>
@@ -3893,21 +3906,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AMJ92"/>
   <sheetViews>
     <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="35.36328125" style="1" customWidth="1"/>
-    <col min="3" max="64" width="8.1796875" customWidth="1"/>
-    <col min="65" max="1024" width="10.54296875" style="1"/>
+    <col min="1" max="2" width="35.42578125" style="1" customWidth="1"/>
+    <col min="3" max="64" width="8.140625" customWidth="1"/>
+    <col min="65" max="1024" width="10.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>80</v>
       </c>
@@ -3915,7 +3928,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>82</v>
       </c>
@@ -3923,7 +3936,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>84</v>
       </c>
@@ -3931,7 +3944,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>86</v>
       </c>
@@ -3939,7 +3952,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>88</v>
       </c>
@@ -3947,7 +3960,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>89</v>
       </c>
@@ -3955,7 +3968,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>91</v>
       </c>
@@ -3963,7 +3976,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>92</v>
       </c>
@@ -3971,7 +3984,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>94</v>
       </c>
@@ -3979,7 +3992,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>96</v>
       </c>
@@ -3987,7 +4000,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>98</v>
       </c>
@@ -3995,7 +4008,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>100</v>
       </c>
@@ -4003,7 +4016,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>102</v>
       </c>
@@ -4011,7 +4024,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>104</v>
       </c>
@@ -4019,7 +4032,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>106</v>
       </c>
@@ -4027,7 +4040,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>108</v>
       </c>
@@ -4035,7 +4048,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>110</v>
       </c>
@@ -4043,7 +4056,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>111</v>
       </c>
@@ -4051,7 +4064,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>112</v>
       </c>
@@ -4059,7 +4072,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>114</v>
       </c>
@@ -4067,7 +4080,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>116</v>
       </c>
@@ -4075,7 +4088,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>117</v>
       </c>
@@ -4083,7 +4096,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>118</v>
       </c>
@@ -4091,7 +4104,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>119</v>
       </c>
@@ -4099,7 +4112,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>120</v>
       </c>
@@ -4107,7 +4120,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>121</v>
       </c>
@@ -4115,7 +4128,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>83</v>
       </c>
@@ -4123,7 +4136,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>122</v>
       </c>
@@ -4131,7 +4144,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>124</v>
       </c>
@@ -4139,7 +4152,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>125</v>
       </c>
@@ -4147,7 +4160,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>127</v>
       </c>
@@ -4155,7 +4168,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>129</v>
       </c>
@@ -4163,7 +4176,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>131</v>
       </c>
@@ -4171,7 +4184,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>133</v>
       </c>
@@ -4179,7 +4192,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>135</v>
       </c>
@@ -4187,7 +4200,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>137</v>
       </c>
@@ -4195,7 +4208,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>139</v>
       </c>
@@ -4203,7 +4216,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>141</v>
       </c>
@@ -4211,7 +4224,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>143</v>
       </c>
@@ -4219,7 +4232,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>145</v>
       </c>
@@ -4227,7 +4240,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>147</v>
       </c>
@@ -4235,7 +4248,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>149</v>
       </c>
@@ -4243,7 +4256,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>151</v>
       </c>
@@ -4251,7 +4264,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>153</v>
       </c>
@@ -4259,7 +4272,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>155</v>
       </c>
@@ -4267,7 +4280,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>157</v>
       </c>
@@ -4275,7 +4288,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>159</v>
       </c>
@@ -4283,7 +4296,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>160</v>
       </c>
@@ -4291,7 +4304,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>161</v>
       </c>
@@ -4299,7 +4312,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>163</v>
       </c>
@@ -4307,7 +4320,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>165</v>
       </c>
@@ -4315,7 +4328,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>167</v>
       </c>
@@ -4323,7 +4336,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>166</v>
       </c>
@@ -4331,7 +4344,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>169</v>
       </c>
@@ -4339,7 +4352,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>171</v>
       </c>
@@ -4347,7 +4360,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>173</v>
       </c>
@@ -4355,7 +4368,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>174</v>
       </c>
@@ -4363,7 +4376,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>175</v>
       </c>
@@ -4371,7 +4384,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>177</v>
       </c>
@@ -4379,7 +4392,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>178</v>
       </c>
@@ -4387,7 +4400,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>180</v>
       </c>
@@ -4395,7 +4408,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>181</v>
       </c>
@@ -4403,7 +4416,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>183</v>
       </c>
@@ -4411,7 +4424,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>185</v>
       </c>
@@ -4419,7 +4432,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>187</v>
       </c>
@@ -4427,7 +4440,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>189</v>
       </c>
@@ -4435,7 +4448,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>191</v>
       </c>
@@ -4443,7 +4456,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>193</v>
       </c>
@@ -4451,7 +4464,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>194</v>
       </c>
@@ -4459,7 +4472,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>195</v>
       </c>
@@ -4467,7 +4480,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>196</v>
       </c>
@@ -4475,7 +4488,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>198</v>
       </c>
@@ -4483,7 +4496,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>199</v>
       </c>
@@ -4491,7 +4504,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>201</v>
       </c>
@@ -4499,7 +4512,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>203</v>
       </c>
@@ -4507,7 +4520,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>205</v>
       </c>
@@ -4515,7 +4528,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>207</v>
       </c>
@@ -4523,7 +4536,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>208</v>
       </c>
@@ -4531,7 +4544,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>209</v>
       </c>
@@ -4539,7 +4552,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>211</v>
       </c>
@@ -4547,7 +4560,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>213</v>
       </c>
@@ -4555,7 +4568,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>214</v>
       </c>
@@ -4563,7 +4576,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>216</v>
       </c>
@@ -4571,7 +4584,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>217</v>
       </c>
@@ -4579,7 +4592,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>219</v>
       </c>
@@ -4587,7 +4600,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>221</v>
       </c>
@@ -4595,7 +4608,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>223</v>
       </c>
@@ -4603,7 +4616,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>224</v>
       </c>
@@ -4611,7 +4624,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>226</v>
       </c>
@@ -4619,7 +4632,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>228</v>
       </c>
@@ -4627,12 +4640,12 @@
         <v>229</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>999</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>99</v>
       </c>
@@ -4648,23 +4661,23 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AMJ157"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.54296875" style="1" customWidth="1"/>
-    <col min="4" max="64" width="8.1796875" customWidth="1"/>
-    <col min="65" max="1024" width="10.54296875" style="1"/>
+    <col min="1" max="1" width="17.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" style="1" customWidth="1"/>
+    <col min="4" max="64" width="8.140625" customWidth="1"/>
+    <col min="65" max="1024" width="10.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>230</v>
       </c>
@@ -4675,7 +4688,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>232</v>
       </c>
@@ -4686,7 +4699,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>235</v>
       </c>
@@ -4697,7 +4710,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>235</v>
       </c>
@@ -4708,7 +4721,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>239</v>
       </c>
@@ -4719,7 +4732,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>242</v>
       </c>
@@ -4730,7 +4743,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>245</v>
       </c>
@@ -4741,7 +4754,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>245</v>
       </c>
@@ -4752,7 +4765,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>245</v>
       </c>
@@ -4763,7 +4776,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>252</v>
       </c>
@@ -4774,7 +4787,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>252</v>
       </c>
@@ -4785,7 +4798,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>252</v>
       </c>
@@ -4796,7 +4809,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>252</v>
       </c>
@@ -4807,7 +4820,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>252</v>
       </c>
@@ -4818,7 +4831,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>252</v>
       </c>
@@ -4829,7 +4842,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>252</v>
       </c>
@@ -4840,7 +4853,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>252</v>
       </c>
@@ -4851,7 +4864,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>269</v>
       </c>
@@ -4862,7 +4875,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>269</v>
       </c>
@@ -4873,7 +4886,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>274</v>
       </c>
@@ -4884,7 +4897,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>277</v>
       </c>
@@ -4895,7 +4908,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>277</v>
       </c>
@@ -4906,7 +4919,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>277</v>
       </c>
@@ -4917,7 +4930,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>277</v>
       </c>
@@ -4928,7 +4941,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>277</v>
       </c>
@@ -4939,7 +4952,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>277</v>
       </c>
@@ -4950,7 +4963,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>277</v>
       </c>
@@ -4961,7 +4974,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>277</v>
       </c>
@@ -4972,7 +4985,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>277</v>
       </c>
@@ -4983,7 +4996,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>277</v>
       </c>
@@ -4994,7 +5007,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>277</v>
       </c>
@@ -5005,7 +5018,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>277</v>
       </c>
@@ -5016,7 +5029,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>277</v>
       </c>
@@ -5027,7 +5040,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>277</v>
       </c>
@@ -5038,7 +5051,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>305</v>
       </c>
@@ -5049,7 +5062,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>305</v>
       </c>
@@ -5060,7 +5073,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>305</v>
       </c>
@@ -5071,7 +5084,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>312</v>
       </c>
@@ -5082,7 +5095,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>312</v>
       </c>
@@ -5093,7 +5106,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>312</v>
       </c>
@@ -5104,7 +5117,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>312</v>
       </c>
@@ -5115,7 +5128,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>321</v>
       </c>
@@ -5126,7 +5139,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>321</v>
       </c>
@@ -5137,7 +5150,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>321</v>
       </c>
@@ -5148,7 +5161,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>321</v>
       </c>
@@ -5159,7 +5172,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>321</v>
       </c>
@@ -5170,7 +5183,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>321</v>
       </c>
@@ -5181,7 +5194,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>321</v>
       </c>
@@ -5192,7 +5205,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>321</v>
       </c>
@@ -5203,7 +5216,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>321</v>
       </c>
@@ -5214,7 +5227,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>336</v>
       </c>
@@ -5225,7 +5238,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>336</v>
       </c>
@@ -5236,7 +5249,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>336</v>
       </c>
@@ -5247,7 +5260,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>336</v>
       </c>
@@ -5258,7 +5271,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>336</v>
       </c>
@@ -5269,7 +5282,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>336</v>
       </c>
@@ -5280,7 +5293,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>336</v>
       </c>
@@ -5291,7 +5304,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>336</v>
       </c>
@@ -5302,7 +5315,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>336</v>
       </c>
@@ -5313,7 +5326,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>336</v>
       </c>
@@ -5324,7 +5337,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>357</v>
       </c>
@@ -5335,7 +5348,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>357</v>
       </c>
@@ -5346,7 +5359,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>357</v>
       </c>
@@ -5357,7 +5370,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>357</v>
       </c>
@@ -5368,7 +5381,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>357</v>
       </c>
@@ -5379,7 +5392,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>357</v>
       </c>
@@ -5390,7 +5403,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>368</v>
       </c>
@@ -5401,7 +5414,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>368</v>
       </c>
@@ -5412,7 +5425,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>368</v>
       </c>
@@ -5423,7 +5436,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>368</v>
       </c>
@@ -5434,7 +5447,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>368</v>
       </c>
@@ -5445,7 +5458,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>368</v>
       </c>
@@ -5456,7 +5469,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>368</v>
       </c>
@@ -5467,7 +5480,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>368</v>
       </c>
@@ -5478,7 +5491,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>368</v>
       </c>
@@ -5489,7 +5502,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>368</v>
       </c>
@@ -5500,7 +5513,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>368</v>
       </c>
@@ -5511,7 +5524,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>368</v>
       </c>
@@ -5522,7 +5535,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>368</v>
       </c>
@@ -5533,7 +5546,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>368</v>
       </c>
@@ -5544,7 +5557,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>368</v>
       </c>
@@ -5555,7 +5568,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>368</v>
       </c>
@@ -5566,7 +5579,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>368</v>
       </c>
@@ -5577,7 +5590,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>368</v>
       </c>
@@ -5588,7 +5601,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>368</v>
       </c>
@@ -5599,7 +5612,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>368</v>
       </c>
@@ -5610,7 +5623,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>368</v>
       </c>
@@ -5621,7 +5634,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>368</v>
       </c>
@@ -5632,7 +5645,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>368</v>
       </c>
@@ -5643,7 +5656,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>368</v>
       </c>
@@ -5654,7 +5667,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>368</v>
       </c>
@@ -5665,7 +5678,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>368</v>
       </c>
@@ -5676,7 +5689,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>368</v>
       </c>
@@ -5687,7 +5700,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>368</v>
       </c>
@@ -5698,7 +5711,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>368</v>
       </c>
@@ -5709,7 +5722,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>427</v>
       </c>
@@ -5720,7 +5733,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>427</v>
       </c>
@@ -5731,7 +5744,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>427</v>
       </c>
@@ -5742,7 +5755,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>427</v>
       </c>
@@ -5753,7 +5766,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>427</v>
       </c>
@@ -5764,7 +5777,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>427</v>
       </c>
@@ -5775,7 +5788,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>427</v>
       </c>
@@ -5786,7 +5799,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>427</v>
       </c>
@@ -5797,7 +5810,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>427</v>
       </c>
@@ -5808,7 +5821,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>427</v>
       </c>
@@ -5819,7 +5832,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>448</v>
       </c>
@@ -5830,7 +5843,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>451</v>
       </c>
@@ -5841,7 +5854,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>451</v>
       </c>
@@ -5852,7 +5865,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>456</v>
       </c>
@@ -5863,7 +5876,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>456</v>
       </c>
@@ -5874,7 +5887,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>456</v>
       </c>
@@ -5885,7 +5898,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>456</v>
       </c>
@@ -5896,7 +5909,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>456</v>
       </c>
@@ -5907,7 +5920,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>464</v>
       </c>
@@ -5918,7 +5931,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>464</v>
       </c>
@@ -5929,7 +5942,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>469</v>
       </c>
@@ -5940,7 +5953,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>469</v>
       </c>
@@ -5951,7 +5964,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>469</v>
       </c>
@@ -5962,7 +5975,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>469</v>
       </c>
@@ -5973,7 +5986,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>469</v>
       </c>
@@ -5984,7 +5997,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>476</v>
       </c>
@@ -5995,7 +6008,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>479</v>
       </c>
@@ -6006,7 +6019,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>479</v>
       </c>
@@ -6017,7 +6030,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>479</v>
       </c>
@@ -6028,7 +6041,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>486</v>
       </c>
@@ -6039,7 +6052,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>486</v>
       </c>
@@ -6050,7 +6063,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>486</v>
       </c>
@@ -6061,7 +6074,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>486</v>
       </c>
@@ -6072,7 +6085,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>486</v>
       </c>
@@ -6083,7 +6096,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>495</v>
       </c>
@@ -6094,7 +6107,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>498</v>
       </c>
@@ -6105,7 +6118,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>70</v>
       </c>
@@ -6116,7 +6129,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>70</v>
       </c>
@@ -6127,7 +6140,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>70</v>
       </c>
@@ -6138,7 +6151,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>70</v>
       </c>
@@ -6149,7 +6162,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>506</v>
       </c>
@@ -6160,7 +6173,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>506</v>
       </c>
@@ -6171,7 +6184,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>510</v>
       </c>
@@ -6182,7 +6195,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>510</v>
       </c>
@@ -6193,7 +6206,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>515</v>
       </c>
@@ -6204,7 +6217,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>515</v>
       </c>
@@ -6215,7 +6228,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>515</v>
       </c>
@@ -6226,7 +6239,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>515</v>
       </c>
@@ -6237,7 +6250,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>515</v>
       </c>
@@ -6248,7 +6261,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>526</v>
       </c>
@@ -6259,7 +6272,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>529</v>
       </c>
@@ -6270,7 +6283,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>529</v>
       </c>
@@ -6281,7 +6294,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>529</v>
       </c>
@@ -6292,7 +6305,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>529</v>
       </c>
@@ -6303,7 +6316,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>529</v>
       </c>
@@ -6314,7 +6327,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>529</v>
       </c>
@@ -6325,7 +6338,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>529</v>
       </c>
@@ -6336,7 +6349,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>544</v>
       </c>
@@ -6347,7 +6360,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>547</v>
       </c>
@@ -6358,7 +6371,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>274</v>
       </c>
@@ -6369,7 +6382,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>357</v>
       </c>
@@ -6380,7 +6393,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>515</v>
       </c>
@@ -6402,23 +6415,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AMJ82"/>
   <sheetViews>
     <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1796875" style="1" customWidth="1"/>
-    <col min="4" max="64" width="8.1796875" customWidth="1"/>
-    <col min="65" max="1024" width="10.54296875" style="1"/>
+    <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="1" customWidth="1"/>
+    <col min="4" max="64" width="8.140625" customWidth="1"/>
+    <col min="65" max="1024" width="10.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>230</v>
       </c>
@@ -6429,7 +6442,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2"/>
       <c r="B2" s="1" t="s">
         <v>558</v>
@@ -6438,7 +6451,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3"/>
       <c r="B3" s="1" t="s">
         <v>559</v>
@@ -6447,7 +6460,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4"/>
       <c r="B4" s="1" t="s">
         <v>560</v>
@@ -6456,7 +6469,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5"/>
       <c r="B5" s="1" t="s">
         <v>562</v>
@@ -6465,7 +6478,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6"/>
       <c r="B6" s="1" t="s">
         <v>563</v>
@@ -6474,7 +6487,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7"/>
       <c r="B7" s="1" t="s">
         <v>565</v>
@@ -6483,7 +6496,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8"/>
       <c r="B8" s="1" t="s">
         <v>567</v>
@@ -6492,7 +6505,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9"/>
       <c r="B9" s="1" t="s">
         <v>569</v>
@@ -6501,7 +6514,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10"/>
       <c r="B10" s="1" t="s">
         <v>571</v>
@@ -6510,7 +6523,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11"/>
       <c r="B11" s="1" t="s">
         <v>572</v>
@@ -6519,7 +6532,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12"/>
       <c r="B12" s="1" t="s">
         <v>574</v>
@@ -6528,7 +6541,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13"/>
       <c r="B13" s="1" t="s">
         <v>576</v>
@@ -6537,7 +6550,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14"/>
       <c r="B14" s="1" t="s">
         <v>577</v>
@@ -6546,7 +6559,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15"/>
       <c r="B15" s="1" t="s">
         <v>579</v>
@@ -6555,7 +6568,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16"/>
       <c r="B16" s="1" t="s">
         <v>580</v>
@@ -6564,7 +6577,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17"/>
       <c r="B17" s="1" t="s">
         <v>582</v>
@@ -6573,7 +6586,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18"/>
       <c r="B18" s="1" t="s">
         <v>583</v>
@@ -6582,7 +6595,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19"/>
       <c r="B19" s="1" t="s">
         <v>584</v>
@@ -6591,7 +6604,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20"/>
       <c r="B20" s="1" t="s">
         <v>585</v>
@@ -6600,7 +6613,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21"/>
       <c r="B21" s="1" t="s">
         <v>587</v>
@@ -6609,7 +6622,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22"/>
       <c r="B22" s="1" t="s">
         <v>589</v>
@@ -6618,7 +6631,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23"/>
       <c r="B23" s="1" t="s">
         <v>590</v>
@@ -6627,7 +6640,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24"/>
       <c r="B24" s="1" t="s">
         <v>591</v>
@@ -6636,7 +6649,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25"/>
       <c r="B25" s="1" t="s">
         <v>592</v>
@@ -6645,7 +6658,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26"/>
       <c r="B26" s="1" t="s">
         <v>594</v>
@@ -6654,7 +6667,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27"/>
       <c r="B27" s="1" t="s">
         <v>596</v>
@@ -6663,7 +6676,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28"/>
       <c r="B28" s="1" t="s">
         <v>597</v>
@@ -6672,7 +6685,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29"/>
       <c r="B29" s="1" t="s">
         <v>599</v>
@@ -6681,7 +6694,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30"/>
       <c r="B30" s="1" t="s">
         <v>601</v>
@@ -6690,7 +6703,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31"/>
       <c r="B31" s="1" t="s">
         <v>602</v>
@@ -6699,7 +6712,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32"/>
       <c r="B32" s="1" t="s">
         <v>603</v>
@@ -6708,7 +6721,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33"/>
       <c r="B33" s="1" t="s">
         <v>604</v>
@@ -6717,7 +6730,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34"/>
       <c r="B34" s="1" t="s">
         <v>606</v>
@@ -6726,7 +6739,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35"/>
       <c r="B35" s="1" t="s">
         <v>607</v>
@@ -6735,7 +6748,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36"/>
       <c r="B36" s="1" t="s">
         <v>608</v>
@@ -6744,7 +6757,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37"/>
       <c r="B37" s="1" t="s">
         <v>609</v>
@@ -6753,7 +6766,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38"/>
       <c r="B38" s="1" t="s">
         <v>610</v>
@@ -6762,7 +6775,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39"/>
       <c r="B39" s="1" t="s">
         <v>611</v>
@@ -6771,7 +6784,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40"/>
       <c r="B40" s="1" t="s">
         <v>612</v>
@@ -6780,7 +6793,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41"/>
       <c r="B41" s="1" t="s">
         <v>613</v>
@@ -6789,7 +6802,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42"/>
       <c r="B42" s="1" t="s">
         <v>614</v>
@@ -6798,7 +6811,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43"/>
       <c r="B43" s="1" t="s">
         <v>615</v>
@@ -6807,7 +6820,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44"/>
       <c r="B44" s="1" t="s">
         <v>616</v>
@@ -6816,7 +6829,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45"/>
       <c r="B45" s="1" t="s">
         <v>617</v>
@@ -6825,7 +6838,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46"/>
       <c r="B46" s="1" t="s">
         <v>618</v>
@@ -6834,7 +6847,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47"/>
       <c r="B47" s="1" t="s">
         <v>619</v>
@@ -6843,7 +6856,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48"/>
       <c r="B48" s="1" t="s">
         <v>620</v>
@@ -6852,7 +6865,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49"/>
       <c r="B49" s="1" t="s">
         <v>622</v>
@@ -6861,7 +6874,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50"/>
       <c r="B50" s="1" t="s">
         <v>623</v>
@@ -6870,7 +6883,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51"/>
       <c r="B51" s="1" t="s">
         <v>625</v>
@@ -6879,7 +6892,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52"/>
       <c r="B52" s="1" t="s">
         <v>626</v>
@@ -6888,7 +6901,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53"/>
       <c r="B53" s="1" t="s">
         <v>628</v>
@@ -6897,7 +6910,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54"/>
       <c r="B54" s="1" t="s">
         <v>630</v>
@@ -6906,7 +6919,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55"/>
       <c r="B55" s="1" t="s">
         <v>114</v>
@@ -6915,7 +6928,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56"/>
       <c r="B56" s="1" t="s">
         <v>155</v>
@@ -6924,7 +6937,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57"/>
       <c r="B57" s="1" t="s">
         <v>159</v>
@@ -6933,7 +6946,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58"/>
       <c r="B58" s="1" t="s">
         <v>193</v>
@@ -6942,7 +6955,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59"/>
       <c r="B59" s="1" t="s">
         <v>632</v>
@@ -6951,7 +6964,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60"/>
       <c r="B60" s="1" t="s">
         <v>633</v>
@@ -6960,7 +6973,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61"/>
       <c r="B61" s="1" t="s">
         <v>634</v>
@@ -6969,7 +6982,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62"/>
       <c r="B62" s="1" t="s">
         <v>635</v>
@@ -6978,7 +6991,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63"/>
       <c r="B63" s="1" t="s">
         <v>636</v>
@@ -6987,7 +7000,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64"/>
       <c r="B64" s="1" t="s">
         <v>637</v>
@@ -6996,7 +7009,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65"/>
       <c r="B65" s="1" t="s">
         <v>638</v>
@@ -7005,7 +7018,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66"/>
       <c r="B66" s="1" t="s">
         <v>639</v>
@@ -7014,7 +7027,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67"/>
       <c r="B67" s="1" t="s">
         <v>640</v>
@@ -7023,7 +7036,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68"/>
       <c r="B68" s="1" t="s">
         <v>641</v>
@@ -7032,7 +7045,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69"/>
       <c r="B69" s="1" t="s">
         <v>181</v>
@@ -7041,7 +7054,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70"/>
       <c r="B70" s="1" t="s">
         <v>642</v>
@@ -7050,7 +7063,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71"/>
       <c r="B71" s="1" t="s">
         <v>643</v>
@@ -7059,7 +7072,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72"/>
       <c r="B72" s="1" t="s">
         <v>644</v>
@@ -7068,7 +7081,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73"/>
       <c r="B73" s="1" t="s">
         <v>646</v>
@@ -7077,7 +7090,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74"/>
       <c r="B74" s="1" t="s">
         <v>647</v>
@@ -7086,7 +7099,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75"/>
       <c r="B75" s="1" t="s">
         <v>649</v>
@@ -7095,7 +7108,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>515</v>
       </c>
@@ -7106,7 +7119,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>515</v>
       </c>
@@ -7117,7 +7130,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>515</v>
       </c>
@@ -7128,7 +7141,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>515</v>
       </c>
@@ -7139,7 +7152,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>515</v>
       </c>
@@ -7150,7 +7163,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>515</v>
       </c>
@@ -7158,7 +7171,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B82" s="1">
         <v>99</v>
       </c>
@@ -7174,22 +7187,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:AMJ6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.08984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" style="1" customWidth="1"/>
-    <col min="3" max="64" width="8.1796875" customWidth="1"/>
-    <col min="65" max="1024" width="10.54296875" style="1"/>
+    <col min="1" max="1" width="6.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="1" customWidth="1"/>
+    <col min="3" max="64" width="8.140625" customWidth="1"/>
+    <col min="65" max="1024" width="10.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -7197,7 +7210,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -7205,15 +7218,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>8</v>
       </c>
@@ -7221,12 +7234,20 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
6-10-22 R code for summarized and mics disability + hh_edu
</commit_message>
<xml_diff>
--- a/wide_pipeline/dhs_dictionary_setcode.xlsx
+++ b/wide_pipeline/dhs_dictionary_setcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\personal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F888F3C8-1B78-4DAB-82EF-3EC5625E4F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05830713-5DF3-4DEB-BFEF-19F0B43980EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="672">
   <si>
     <t>name</t>
   </si>
@@ -2025,15 +2025,48 @@
   </si>
   <si>
     <t>hv101</t>
+  </si>
+  <si>
+    <t>hdis1</t>
+  </si>
+  <si>
+    <t>hdis2</t>
+  </si>
+  <si>
+    <t>hdis3</t>
+  </si>
+  <si>
+    <t>hdis4</t>
+  </si>
+  <si>
+    <t>hdis5</t>
+  </si>
+  <si>
+    <t>hdis6</t>
+  </si>
+  <si>
+    <t>hdis7</t>
+  </si>
+  <si>
+    <t>hdis8</t>
+  </si>
+  <si>
+    <t>hdis9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -2345,10 +2378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D33" sqref="D33:D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2654,7 +2687,80 @@
         <v>1</v>
       </c>
     </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>

</xml_diff>